<commit_message>
Update trading results - Fri Sep  5 12:39:27 UTC 2025
</commit_message>
<xml_diff>
--- a/results/momentum_portfolio_simulation_latest.xlsx
+++ b/results/momentum_portfolio_simulation_latest.xlsx
@@ -1678,7 +1678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10028,19 +10028,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>201.9159629811668</v>
+        <v>202.685562461319</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.9806982599722289</v>
+        <v>-0.8203650349405223</v>
       </c>
       <c r="D182" t="n">
-        <v>0.7939285370962909</v>
+        <v>0.7974674083575578</v>
       </c>
       <c r="E182" t="n">
-        <v>-84792438.58563519</v>
+        <v>-124403393.1976814</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -10057,7 +10057,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-1.204976821539826</v>
+        <v>-1.101213139679351</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -10069,52 +10069,6 @@
         <v>20</v>
       </c>
       <c r="N182" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>202.685562461319</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.4361131129962246</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.7978202504400181</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-34697261.66185951</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.8389528062753741</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1400</v>
-      </c>
-      <c r="M183" t="n">
-        <v>20</v>
-      </c>
-      <c r="N183" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11416,7 +11370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19766,19 +19720,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>3.28093499945639</v>
+        <v>3.289019298851818</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.004886243174949012</v>
+        <v>-0.003202014134235043</v>
       </c>
       <c r="D182" t="n">
-        <v>0.01379316754374932</v>
+        <v>0.01384075054053449</v>
       </c>
       <c r="E182" t="n">
-        <v>-6400108.026912928</v>
+        <v>-4900742.48875463</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -19795,7 +19749,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.8308060362753866</v>
+        <v>-0.7585902550635818</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -19807,52 +19761,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>3.289019298851818</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.0001366608816293358</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.01408862025165007</v>
-      </c>
-      <c r="E183" t="n">
-        <v>4443660.398805022</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.636701135947217</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -21154,7 +21062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29504,19 +29412,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>0.33426016433722</v>
+        <v>0.3346362672061652</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.0003125056951998051</v>
+        <v>-0.0002341509308362855</v>
       </c>
       <c r="D182" t="n">
-        <v>0.0003568814270843897</v>
+        <v>0.0003593234949698433</v>
       </c>
       <c r="E182" t="n">
-        <v>11255520.01799738</v>
+        <v>11016877.39325476</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -29533,7 +29441,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.6631562970023621</v>
+        <v>-0.5881480416479171</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -29545,52 +29453,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>0.3346362672061652</v>
-      </c>
-      <c r="C183" t="n">
-        <v>2.393049624038746e-05</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.000356120290371048</v>
-      </c>
-      <c r="E183" t="n">
-        <v>8791663.43144393</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.3291401475258089</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -30800,7 +30662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39150,19 +39012,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>2.786871763078856</v>
+        <v>2.797620314598713</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.00366558314893739</v>
+        <v>-0.001426301582300837</v>
       </c>
       <c r="D182" t="n">
-        <v>0.008919414512336294</v>
+        <v>0.008981888955194384</v>
       </c>
       <c r="E182" t="n">
-        <v>-28217800.47530842</v>
+        <v>-62532405.51299</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -39179,7 +39041,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.8915771376991467</v>
+        <v>-0.7386359407398257</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -39191,52 +39053,6 @@
         <v>20</v>
       </c>
       <c r="N182" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>2.797620314598713</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.00122411678366019</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.009161126425197869</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-27618429.1849699</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.5669858090957896</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1400</v>
-      </c>
-      <c r="M183" t="n">
-        <v>20</v>
-      </c>
-      <c r="N183" t="n">
         <v>20</v>
       </c>
     </row>
@@ -48071,7 +47887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56421,19 +56237,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>0.4838630802815537</v>
+        <v>0.4827101994643042</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.001371782525943444</v>
+        <v>-0.001611966029537115</v>
       </c>
       <c r="D182" t="n">
-        <v>0.002471756307512945</v>
+        <v>0.002464569294048336</v>
       </c>
       <c r="E182" t="n">
-        <v>4400626.81975174</v>
+        <v>1117257.728360713</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -56450,7 +56266,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.6773683269750277</v>
+        <v>-0.7182232419990181</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -56462,52 +56278,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>0.4827101994643042</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.0007199465426226959</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.002500435216852542</v>
-      </c>
-      <c r="E183" t="n">
-        <v>2149123.553186893</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.5680196207051338</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -57533,7 +57303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -65883,19 +65653,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>110677.1951111714</v>
+        <v>110724.736377486</v>
       </c>
       <c r="C182" t="n">
-        <v>-72.34978851435881</v>
+        <v>-62.44535803215695</v>
       </c>
       <c r="D182" t="n">
-        <v>216.204707681023</v>
+        <v>216.4632568086899</v>
       </c>
       <c r="E182" t="n">
-        <v>-88909498.9480896</v>
+        <v>-148040705.2601166</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -65912,7 +65682,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.934687950385557</v>
+        <v>-0.9038621892037123</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -65924,52 +65694,6 @@
         <v>40</v>
       </c>
       <c r="N182" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>110724.736377486</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-37.83565767183609</v>
-      </c>
-      <c r="D183" t="n">
-        <v>218.5515797076512</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-106479308.3833618</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.8346939902385648</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>2800</v>
-      </c>
-      <c r="M183" t="n">
-        <v>40</v>
-      </c>
-      <c r="N183" t="n">
         <v>40</v>
       </c>
     </row>
@@ -67179,7 +66903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -75529,19 +75253,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>4313.093551047387</v>
+        <v>4298.094660544595</v>
       </c>
       <c r="C182" t="n">
-        <v>-4.439933928085338</v>
+        <v>-7.564702782832683</v>
       </c>
       <c r="D182" t="n">
-        <v>15.85995754500211</v>
+        <v>15.76653848388979</v>
       </c>
       <c r="E182" t="n">
-        <v>122153935.8585968</v>
+        <v>-54412393.12631989</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -75558,7 +75282,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.6509830447996358</v>
+        <v>-0.7476782683163902</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -75570,52 +75294,6 @@
         <v>25</v>
       </c>
       <c r="N182" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>4298.094660544595</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-4.188049219074856</v>
-      </c>
-      <c r="D183" t="n">
-        <v>15.84770871178337</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-90851269.91069412</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.6424744330847846</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1750</v>
-      </c>
-      <c r="M183" t="n">
-        <v>25</v>
-      </c>
-      <c r="N183" t="n">
         <v>25</v>
       </c>
     </row>
@@ -76733,7 +76411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -85083,19 +84761,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45905.04166666666</v>
+        <v>45905.5</v>
       </c>
       <c r="B182" t="n">
-        <v>2.373475042044198</v>
+        <v>2.377609123224236</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.005675641927169739</v>
+        <v>-0.004814375014661643</v>
       </c>
       <c r="D182" t="n">
-        <v>0.01038442178366865</v>
+        <v>0.01040677362239898</v>
       </c>
       <c r="E182" t="n">
-        <v>1102746.435115397</v>
+        <v>31517.88170982897</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -85112,7 +84790,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.9526321069067126</v>
+        <v>-0.9035517457119542</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -85124,52 +84802,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45905.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>2.377609123224236</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.00135730363337494</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.01048034146960766</v>
-      </c>
-      <c r="E183" t="n">
-        <v>489670.1410580128</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.7036496499210156</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update trading results - Sat Sep  6 12:35:23 UTC 2025
</commit_message>
<xml_diff>
--- a/results/momentum_portfolio_simulation_latest.xlsx
+++ b/results/momentum_portfolio_simulation_latest.xlsx
@@ -1678,7 +1678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10028,19 +10028,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>203.9131779989764</v>
+        <v>203.479136779819</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.1510746957802382</v>
+        <v>-0.2414999497713666</v>
       </c>
       <c r="D182" t="n">
-        <v>0.7205285345407756</v>
+        <v>0.7177343493736895</v>
       </c>
       <c r="E182" t="n">
-        <v>218863493.497303</v>
+        <v>252826002.4863367</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -10057,7 +10057,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.61051286501394</v>
+        <v>-0.6716868819681535</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -10069,52 +10069,6 @@
         <v>20</v>
       </c>
       <c r="N182" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>203.479136779819</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.1908313323461925</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.5452270443675215</v>
-      </c>
-      <c r="E183" t="n">
-        <v>181764553.4992571</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.5665445469570917</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1400</v>
-      </c>
-      <c r="M183" t="n">
-        <v>20</v>
-      </c>
-      <c r="N183" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11416,7 +11370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19766,19 +19720,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>3.390570456858071</v>
+        <v>3.376056885966955</v>
       </c>
       <c r="C182" t="n">
-        <v>0.01068406419595958</v>
+        <v>0.007660403593643395</v>
       </c>
       <c r="D182" t="n">
-        <v>0.01374564818158755</v>
+        <v>0.01362967755525921</v>
       </c>
       <c r="E182" t="n">
-        <v>38756630.02010953</v>
+        <v>45140423.42724168</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -19795,7 +19749,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.1414587736488042</v>
+        <v>-0.2761944466623787</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -19807,52 +19761,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>3.376056885966955</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.002800482955823025</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.01043904226636248</v>
-      </c>
-      <c r="E183" t="n">
-        <v>28964948.80675638</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.405977181449957</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -21246,7 +21154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29596,19 +29504,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>0.3315601195407648</v>
+        <v>0.3312366536211805</v>
       </c>
       <c r="C182" t="n">
-        <v>-9.546051566899916e-05</v>
+        <v>-0.0001628492489156308</v>
       </c>
       <c r="D182" t="n">
-        <v>0.0002629795304956525</v>
+        <v>0.0002606185778002134</v>
       </c>
       <c r="E182" t="n">
-        <v>23282650.67871225</v>
+        <v>24581876.80342889</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -29625,7 +29533,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.3678945617951754</v>
+        <v>-0.4347398952848179</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -29637,52 +29545,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>0.3312366536211805</v>
-      </c>
-      <c r="C183" t="n">
-        <v>4.351165170862759e-05</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.0001509889118283685</v>
-      </c>
-      <c r="E183" t="n">
-        <v>13706999.69499362</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.1219945723182186</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -30892,7 +30754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39242,19 +39104,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>2.817414145240768</v>
+        <v>2.816094713923012</v>
       </c>
       <c r="C182" t="n">
-        <v>0.002938638160681961</v>
+        <v>0.002663756636149373</v>
       </c>
       <c r="D182" t="n">
-        <v>0.008428881388954531</v>
+        <v>0.008419333030119229</v>
       </c>
       <c r="E182" t="n">
-        <v>172894148.701973</v>
+        <v>183832406.3825712</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -39271,7 +39133,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.4087408193885665</v>
+        <v>-0.4285191031028929</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -39283,52 +39145,6 @@
         <v>20</v>
       </c>
       <c r="N182" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>2.816094713923012</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.002134627596359628</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.006182624838430995</v>
-      </c>
-      <c r="E183" t="n">
-        <v>107555276.6559219</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.3546646753623696</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1400</v>
-      </c>
-      <c r="M183" t="n">
-        <v>20</v>
-      </c>
-      <c r="N183" t="n">
         <v>20</v>
       </c>
     </row>
@@ -48071,7 +47887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56421,19 +56237,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>0.4987983814940565</v>
+        <v>0.4945964674320544</v>
       </c>
       <c r="C182" t="n">
-        <v>0.00185786165079832</v>
+        <v>0.0009824628878812858</v>
       </c>
       <c r="D182" t="n">
-        <v>0.002284194311437943</v>
+        <v>0.002249810726583133</v>
       </c>
       <c r="E182" t="n">
-        <v>15166275.31032085</v>
+        <v>15081081.16156191</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -56450,7 +56266,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.0780749379505028</v>
+        <v>-0.2325344921750002</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -56462,52 +56278,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>0.4945964674320544</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.0003556811470539212</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.001497621794809786</v>
-      </c>
-      <c r="E183" t="n">
-        <v>9631807.2372666</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.2392215602806605</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -57533,7 +57303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -65883,19 +65653,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>110841.0127111492</v>
+        <v>110662.1811262851</v>
       </c>
       <c r="C182" t="n">
-        <v>3.184674756252207</v>
+        <v>-34.07190542375611</v>
       </c>
       <c r="D182" t="n">
-        <v>198.420743512711</v>
+        <v>197.317022067009</v>
       </c>
       <c r="E182" t="n">
-        <v>1382383402.129166</v>
+        <v>1394761690.097931</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -65912,7 +65682,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.654796110677219</v>
+        <v>-0.775329493237164</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -65924,52 +65694,6 @@
         <v>40</v>
       </c>
       <c r="N182" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>110662.1811262851</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-39.02456391628948</v>
-      </c>
-      <c r="D183" t="n">
-        <v>153.7093056032158</v>
-      </c>
-      <c r="E183" t="n">
-        <v>580477110.1963043</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.7305241330781033</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>2800</v>
-      </c>
-      <c r="M183" t="n">
-        <v>40</v>
-      </c>
-      <c r="N183" t="n">
         <v>40</v>
       </c>
     </row>
@@ -67179,7 +66903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -75529,19 +75253,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>4323.826146639187</v>
+        <v>4306.613513100346</v>
       </c>
       <c r="C182" t="n">
-        <v>4.45413585748156</v>
+        <v>0.8681705368890107</v>
       </c>
       <c r="D182" t="n">
-        <v>12.77418849728858</v>
+        <v>12.64525394004064</v>
       </c>
       <c r="E182" t="n">
-        <v>716934149.3626747</v>
+        <v>682373584.270607</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -75558,7 +75282,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.2879820047693997</v>
+        <v>-0.4079057214624144</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -75570,52 +75294,6 @@
         <v>25</v>
       </c>
       <c r="N182" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>4306.613513100346</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.504422986595273</v>
-      </c>
-      <c r="D183" t="n">
-        <v>5.92941449471975</v>
-      </c>
-      <c r="E183" t="n">
-        <v>287119474.2900887</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.2491925444806059</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1750</v>
-      </c>
-      <c r="M183" t="n">
-        <v>25</v>
-      </c>
-      <c r="N183" t="n">
         <v>25</v>
       </c>
     </row>
@@ -76733,7 +76411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -85083,19 +84761,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45906.04166666666</v>
+        <v>45906.5</v>
       </c>
       <c r="B182" t="n">
-        <v>2.402674769599895</v>
+        <v>2.398202970804881</v>
       </c>
       <c r="C182" t="n">
-        <v>0.002740933251800914</v>
+        <v>0.00180930850283989</v>
       </c>
       <c r="D182" t="n">
-        <v>0.009553054627742365</v>
+        <v>0.009521193921504377</v>
       </c>
       <c r="E182" t="n">
-        <v>7184121.702139258</v>
+        <v>7485070.812060624</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -85112,7 +84790,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.4219014550718789</v>
+        <v>-0.4776751014923436</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -85124,52 +84802,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45906.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>2.398202970804881</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.001455202169728942</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.007122075291860832</v>
-      </c>
-      <c r="E183" t="n">
-        <v>4313995.566973776</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.4025304953397368</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update trading results - Sun Sep  7 12:36:11 UTC 2025
</commit_message>
<xml_diff>
--- a/results/momentum_portfolio_simulation_latest.xlsx
+++ b/results/momentum_portfolio_simulation_latest.xlsx
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>303.4196667943351</v>
+        <v>305.6337733039697</v>
       </c>
     </row>
     <row r="8">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>68.53932584269663</v>
+        <v>69.31818181818183</v>
       </c>
     </row>
     <row r="10">
@@ -1678,7 +1678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10028,19 +10028,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>201.8631361529925</v>
+        <v>200.1866593703589</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.01227359558330932</v>
+        <v>-0.361539591965311</v>
       </c>
       <c r="D182" t="n">
-        <v>0.413504350912832</v>
+        <v>0.4017451776498596</v>
       </c>
       <c r="E182" t="n">
-        <v>-264183364.3175449</v>
+        <v>-269696977.5713015</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -10057,7 +10057,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.344134808131997</v>
+        <v>-0.6170412004965763</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -10069,52 +10069,6 @@
         <v>20</v>
       </c>
       <c r="N182" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>200.1866593703589</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.321880119104577</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.3379386809118456</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-86307736.68577242</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.5497894842424165</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1400</v>
-      </c>
-      <c r="M183" t="n">
-        <v>20</v>
-      </c>
-      <c r="N183" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11324,7 +11278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19674,19 +19628,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>3.366106914316116</v>
+        <v>3.336702463994142</v>
       </c>
       <c r="C182" t="n">
-        <v>0.004858789406982478</v>
+        <v>-0.001267137743428126</v>
       </c>
       <c r="D182" t="n">
-        <v>0.00856052590737295</v>
+        <v>0.008343179741690167</v>
       </c>
       <c r="E182" t="n">
-        <v>-58098108.94863319</v>
+        <v>-42354145.3345089</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -19703,7 +19657,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.2086841949332314</v>
+        <v>-0.5425829088005927</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -19715,52 +19669,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>3.336702463994142</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.003516614706313259</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.007772230460118366</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-9606714.708481312</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.6461325591010151</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -21062,7 +20970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29412,36 +29320,36 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>0.3216427903077298</v>
+        <v>0.314521276349756</v>
       </c>
       <c r="C182" t="n">
-        <v>0.0003118801705139229</v>
+        <v>-0.001171768570730591</v>
       </c>
       <c r="D182" t="n">
-        <v>5.643576098979714e-05</v>
+        <v>5.941636238053537e-06</v>
       </c>
       <c r="E182" t="n">
-        <v>80256602.02696991</v>
+        <v>31299176.86613083</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>HOLD</t>
         </is>
       </c>
       <c r="G182" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H182" t="n">
-        <v>0.3216427903077298</v>
+        <v>0</v>
       </c>
       <c r="I182" t="n">
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>0.2542080468227055</v>
+        <v>-1.174439097425514</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -29453,52 +29361,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>0.314521276349756</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-0.0009640236801865543</v>
-      </c>
-      <c r="D183" t="n">
-        <v>3.735276289941681e-05</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-10653029.83301425</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>-2.21410650963459</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.9924478628401808</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -29513,7 +29375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30694,98 +30556,6 @@
         <v>10</v>
       </c>
       <c r="N25" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>45907.04166666666</v>
-      </c>
-      <c r="B26" t="n">
-        <v>0.3216427903077298</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.0003118801705139229</v>
-      </c>
-      <c r="D26" t="n">
-        <v>5.643576098979714e-05</v>
-      </c>
-      <c r="E26" t="n">
-        <v>80256602.02696991</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.3216427903077298</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.2542080468227055</v>
-      </c>
-      <c r="K26" t="n">
-        <v>1</v>
-      </c>
-      <c r="L26" t="n">
-        <v>700</v>
-      </c>
-      <c r="M26" t="n">
-        <v>10</v>
-      </c>
-      <c r="N26" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B27" t="n">
-        <v>0.314521276349756</v>
-      </c>
-      <c r="C27" t="n">
-        <v>-0.0009640236801865543</v>
-      </c>
-      <c r="D27" t="n">
-        <v>3.735276289941681e-05</v>
-      </c>
-      <c r="E27" t="n">
-        <v>-10653029.83301425</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="G27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" t="n">
-        <v>-2.21410650963459</v>
-      </c>
-      <c r="J27" t="n">
-        <v>-0.9924478628401808</v>
-      </c>
-      <c r="K27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" t="n">
-        <v>700</v>
-      </c>
-      <c r="M27" t="n">
-        <v>10</v>
-      </c>
-      <c r="N27" t="n">
         <v>10</v>
       </c>
     </row>
@@ -30800,7 +30570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39150,19 +38920,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>2.820628489966447</v>
+        <v>2.810651604452461</v>
       </c>
       <c r="C182" t="n">
-        <v>0.003559922617296873</v>
+        <v>0.00148140480188319</v>
       </c>
       <c r="D182" t="n">
-        <v>0.005198533811741598</v>
+        <v>0.005120152107312538</v>
       </c>
       <c r="E182" t="n">
-        <v>-335983834.3387036</v>
+        <v>-340062001.6319251</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -39179,7 +38949,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.1527169951685402</v>
+        <v>-0.3397038391570589</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -39191,52 +38961,6 @@
         <v>20</v>
       </c>
       <c r="N182" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>2.810651604452461</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.000522384112551677</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.004804715929138541</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-142857043.3059459</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.4053884804249014</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1400</v>
-      </c>
-      <c r="M183" t="n">
-        <v>20</v>
-      </c>
-      <c r="N183" t="n">
         <v>20</v>
       </c>
     </row>
@@ -40170,7 +39894,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L179"/>
+  <dimension ref="A1:L177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46879,11 +46603,11 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="B160" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45824.5</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
@@ -46891,41 +46615,41 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>0.3216427903077298</v>
+        <v>2.210927953443365</v>
       </c>
       <c r="E160" t="n">
         <v>0</v>
       </c>
       <c r="F160" t="n">
-        <v>0.0003118801705139229</v>
+        <v>0.0136699482316045</v>
       </c>
       <c r="G160" t="n">
-        <v>5.643576098979714e-05</v>
+        <v>0.001894620135573048</v>
       </c>
       <c r="H160" t="n">
-        <v>80256602.02696991</v>
+        <v>250453897.7312098</v>
       </c>
       <c r="I160" t="n">
-        <v>0.2542080468227055</v>
+        <v>1.165876364299861</v>
       </c>
       <c r="J160" t="n">
         <v>1</v>
       </c>
       <c r="K160" t="n">
-        <v>700</v>
+        <v>1400</v>
       </c>
       <c r="L160" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>TRX</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="B161" s="2" t="n">
-        <v>45907.5</v>
+        <v>45826</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
@@ -46933,31 +46657,31 @@
         </is>
       </c>
       <c r="D161" t="n">
-        <v>0.314521276349756</v>
+        <v>2.163231775939699</v>
       </c>
       <c r="E161" t="n">
-        <v>-2.21410650963459</v>
+        <v>-2.157292255018163</v>
       </c>
       <c r="F161" t="n">
-        <v>-0.0009640236801865543</v>
+        <v>-0.009207133260662026</v>
       </c>
       <c r="G161" t="n">
-        <v>3.735276289941681e-05</v>
+        <v>0.003274879058318401</v>
       </c>
       <c r="H161" t="n">
-        <v>-10653029.83301425</v>
+        <v>-29889895.43114567</v>
       </c>
       <c r="I161" t="n">
-        <v>-0.9924478628401808</v>
+        <v>-1.175586807427908</v>
       </c>
       <c r="J161" t="n">
         <v>1</v>
       </c>
       <c r="K161" t="n">
-        <v>700</v>
+        <v>1400</v>
       </c>
       <c r="L161" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162">
@@ -46967,7 +46691,7 @@
         </is>
       </c>
       <c r="B162" s="2" t="n">
-        <v>45824.5</v>
+        <v>45831.5</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
@@ -46975,22 +46699,22 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>2.210927953443365</v>
+        <v>2.088760137377982</v>
       </c>
       <c r="E162" t="n">
         <v>0</v>
       </c>
       <c r="F162" t="n">
-        <v>0.0136699482316045</v>
+        <v>0.01486492966859476</v>
       </c>
       <c r="G162" t="n">
-        <v>0.001894620135573048</v>
+        <v>0.002000568490001819</v>
       </c>
       <c r="H162" t="n">
-        <v>250453897.7312098</v>
+        <v>154715761.447947</v>
       </c>
       <c r="I162" t="n">
-        <v>1.165876364299861</v>
+        <v>1.376268541052534</v>
       </c>
       <c r="J162" t="n">
         <v>1</v>
@@ -47009,30 +46733,30 @@
         </is>
       </c>
       <c r="B163" s="2" t="n">
-        <v>45826</v>
+        <v>45833.5</v>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>SELL_VOLUME</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>2.163231775939699</v>
+        <v>2.186476900305086</v>
       </c>
       <c r="E163" t="n">
-        <v>-2.157292255018163</v>
+        <v>4.678218488493711</v>
       </c>
       <c r="F163" t="n">
-        <v>-0.009207133260662026</v>
+        <v>0.00699565744403996</v>
       </c>
       <c r="G163" t="n">
-        <v>0.003274879058318401</v>
+        <v>0.004648952851787541</v>
       </c>
       <c r="H163" t="n">
-        <v>-29889895.43114567</v>
+        <v>-210695661.8755474</v>
       </c>
       <c r="I163" t="n">
-        <v>-1.175586807427908</v>
+        <v>0.2105809520918032</v>
       </c>
       <c r="J163" t="n">
         <v>1</v>
@@ -47051,7 +46775,7 @@
         </is>
       </c>
       <c r="B164" s="2" t="n">
-        <v>45831.5</v>
+        <v>45847.5</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
@@ -47059,22 +46783,22 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>2.088760137377982</v>
+        <v>2.357941413071812</v>
       </c>
       <c r="E164" t="n">
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>0.01486492966859476</v>
+        <v>0.01104274758703472</v>
       </c>
       <c r="G164" t="n">
-        <v>0.002000568490001819</v>
+        <v>0.004751304362618442</v>
       </c>
       <c r="H164" t="n">
-        <v>154715761.447947</v>
+        <v>114060796.6551976</v>
       </c>
       <c r="I164" t="n">
-        <v>1.376268541052534</v>
+        <v>0.9926221336101746</v>
       </c>
       <c r="J164" t="n">
         <v>1</v>
@@ -47093,30 +46817,30 @@
         </is>
       </c>
       <c r="B165" s="2" t="n">
-        <v>45833.5</v>
+        <v>45853.5</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>SELL_VOLUME</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>2.186476900305086</v>
+        <v>2.936004628778936</v>
       </c>
       <c r="E165" t="n">
-        <v>4.678218488493711</v>
+        <v>24.51558857664965</v>
       </c>
       <c r="F165" t="n">
-        <v>0.00699565744403996</v>
+        <v>-0.007133683517837053</v>
       </c>
       <c r="G165" t="n">
-        <v>0.004648952851787541</v>
+        <v>0.01051482515638282</v>
       </c>
       <c r="H165" t="n">
-        <v>-210695661.8755474</v>
+        <v>-145106084.5385532</v>
       </c>
       <c r="I165" t="n">
-        <v>0.2105809520918032</v>
+        <v>-1.72983710136922</v>
       </c>
       <c r="J165" t="n">
         <v>1</v>
@@ -47135,7 +46859,7 @@
         </is>
       </c>
       <c r="B166" s="2" t="n">
-        <v>45847.5</v>
+        <v>45855.5</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
@@ -47143,22 +46867,22 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>2.357941413071812</v>
+        <v>3.267675369404749</v>
       </c>
       <c r="E166" t="n">
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>0.01104274758703472</v>
+        <v>0.04200698692475369</v>
       </c>
       <c r="G166" t="n">
-        <v>0.004751304362618442</v>
+        <v>0.01285608175063692</v>
       </c>
       <c r="H166" t="n">
-        <v>114060796.6551976</v>
+        <v>1081654140.701865</v>
       </c>
       <c r="I166" t="n">
-        <v>0.9926221336101746</v>
+        <v>2.364119103648554</v>
       </c>
       <c r="J166" t="n">
         <v>1</v>
@@ -47177,7 +46901,7 @@
         </is>
       </c>
       <c r="B167" s="2" t="n">
-        <v>45853.5</v>
+        <v>45857</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
@@ -47185,22 +46909,22 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>2.936004628778936</v>
+        <v>3.417044710420229</v>
       </c>
       <c r="E167" t="n">
-        <v>24.51558857664965</v>
+        <v>4.571119347228472</v>
       </c>
       <c r="F167" t="n">
-        <v>-0.007133683517837053</v>
+        <v>-0.01058440673957328</v>
       </c>
       <c r="G167" t="n">
-        <v>0.01051482515638282</v>
+        <v>0.01674953301728384</v>
       </c>
       <c r="H167" t="n">
-        <v>-145106084.5385532</v>
+        <v>-200365495.2610607</v>
       </c>
       <c r="I167" t="n">
-        <v>-1.72983710136922</v>
+        <v>-1.662853534058789</v>
       </c>
       <c r="J167" t="n">
         <v>1</v>
@@ -47219,7 +46943,7 @@
         </is>
       </c>
       <c r="B168" s="2" t="n">
-        <v>45855.5</v>
+        <v>45876.5</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
@@ -47227,22 +46951,22 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>3.267675369404749</v>
+        <v>3.153739489446899</v>
       </c>
       <c r="E168" t="n">
         <v>0</v>
       </c>
       <c r="F168" t="n">
-        <v>0.04200698692475369</v>
+        <v>0.03691217959442561</v>
       </c>
       <c r="G168" t="n">
-        <v>0.01285608175063692</v>
+        <v>0.008503144743068016</v>
       </c>
       <c r="H168" t="n">
-        <v>1081654140.701865</v>
+        <v>359580240.767417</v>
       </c>
       <c r="I168" t="n">
-        <v>2.364119103648554</v>
+        <v>1.201627714096317</v>
       </c>
       <c r="J168" t="n">
         <v>1</v>
@@ -47261,7 +46985,7 @@
         </is>
       </c>
       <c r="B169" s="2" t="n">
-        <v>45857</v>
+        <v>45878.5</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
@@ -47269,22 +46993,22 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>3.417044710420229</v>
+        <v>3.258835895366054</v>
       </c>
       <c r="E169" t="n">
-        <v>4.571119347228472</v>
+        <v>3.332437770171912</v>
       </c>
       <c r="F169" t="n">
-        <v>-0.01058440673957328</v>
+        <v>-0.005970649058068656</v>
       </c>
       <c r="G169" t="n">
-        <v>0.01674953301728384</v>
+        <v>0.01449355259858687</v>
       </c>
       <c r="H169" t="n">
-        <v>-200365495.2610607</v>
+        <v>-253941684.227375</v>
       </c>
       <c r="I169" t="n">
-        <v>-1.662853534058789</v>
+        <v>-1.109079275986783</v>
       </c>
       <c r="J169" t="n">
         <v>1</v>
@@ -47303,7 +47027,7 @@
         </is>
       </c>
       <c r="B170" s="2" t="n">
-        <v>45876.5</v>
+        <v>45882</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
@@ -47311,22 +47035,22 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>3.153739489446899</v>
+        <v>3.26747236546907</v>
       </c>
       <c r="E170" t="n">
         <v>0</v>
       </c>
       <c r="F170" t="n">
-        <v>0.03691217959442561</v>
+        <v>0.01407219190853182</v>
       </c>
       <c r="G170" t="n">
-        <v>0.008503144743068016</v>
+        <v>0.01253020871461937</v>
       </c>
       <c r="H170" t="n">
-        <v>359580240.767417</v>
+        <v>298849571.1437731</v>
       </c>
       <c r="I170" t="n">
-        <v>1.201627714096317</v>
+        <v>0.0778418750195686</v>
       </c>
       <c r="J170" t="n">
         <v>1</v>
@@ -47345,7 +47069,7 @@
         </is>
       </c>
       <c r="B171" s="2" t="n">
-        <v>45878.5</v>
+        <v>45883.5</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
@@ -47353,22 +47077,22 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>3.258835895366054</v>
+        <v>3.186945905201149</v>
       </c>
       <c r="E171" t="n">
-        <v>3.332437770171912</v>
+        <v>-2.464487875059974</v>
       </c>
       <c r="F171" t="n">
-        <v>-0.005970649058068656</v>
+        <v>-0.02001160819109327</v>
       </c>
       <c r="G171" t="n">
-        <v>0.01449355259858687</v>
+        <v>0.01270242921170287</v>
       </c>
       <c r="H171" t="n">
-        <v>-253941684.227375</v>
+        <v>303885835.3385611</v>
       </c>
       <c r="I171" t="n">
-        <v>-1.109079275986783</v>
+        <v>-1.617132562699669</v>
       </c>
       <c r="J171" t="n">
         <v>1</v>
@@ -47387,7 +47111,7 @@
         </is>
       </c>
       <c r="B172" s="2" t="n">
-        <v>45882</v>
+        <v>45890</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -47395,22 +47119,22 @@
         </is>
       </c>
       <c r="D172" t="n">
-        <v>3.26747236546907</v>
+        <v>2.952309340790555</v>
       </c>
       <c r="E172" t="n">
         <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>0.01407219190853182</v>
+        <v>0.01082555663730611</v>
       </c>
       <c r="G172" t="n">
-        <v>0.01253020871461937</v>
+        <v>0.007441877724894171</v>
       </c>
       <c r="H172" t="n">
-        <v>298849571.1437731</v>
+        <v>43827841.31850338</v>
       </c>
       <c r="I172" t="n">
-        <v>0.0778418750195686</v>
+        <v>0.1792525538946588</v>
       </c>
       <c r="J172" t="n">
         <v>1</v>
@@ -47429,7 +47153,7 @@
         </is>
       </c>
       <c r="B173" s="2" t="n">
-        <v>45883.5</v>
+        <v>45890.5</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
@@ -47437,22 +47161,22 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>3.186945905201149</v>
+        <v>2.901066174357815</v>
       </c>
       <c r="E173" t="n">
-        <v>-2.464487875059974</v>
+        <v>-1.735697737521566</v>
       </c>
       <c r="F173" t="n">
-        <v>-0.02001160819109327</v>
+        <v>-0.0009501258603874518</v>
       </c>
       <c r="G173" t="n">
-        <v>0.01270242921170287</v>
+        <v>0.007367844180052161</v>
       </c>
       <c r="H173" t="n">
-        <v>303885835.3385611</v>
+        <v>-228659661.1411896</v>
       </c>
       <c r="I173" t="n">
-        <v>-1.617132562699669</v>
+        <v>-0.4408405543264862</v>
       </c>
       <c r="J173" t="n">
         <v>1</v>
@@ -47471,7 +47195,7 @@
         </is>
       </c>
       <c r="B174" s="2" t="n">
-        <v>45890</v>
+        <v>45891.5</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
@@ -47479,22 +47203,22 @@
         </is>
       </c>
       <c r="D174" t="n">
-        <v>2.952309340790555</v>
+        <v>2.961548895020256</v>
       </c>
       <c r="E174" t="n">
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>0.01082555663730611</v>
+        <v>0.02251244456848189</v>
       </c>
       <c r="G174" t="n">
-        <v>0.007441877724894171</v>
+        <v>0.006040177084133864</v>
       </c>
       <c r="H174" t="n">
-        <v>43827841.31850338</v>
+        <v>349435963.2458496</v>
       </c>
       <c r="I174" t="n">
-        <v>0.1792525538946588</v>
+        <v>0.9160404318878156</v>
       </c>
       <c r="J174" t="n">
         <v>1</v>
@@ -47513,30 +47237,30 @@
         </is>
       </c>
       <c r="B175" s="2" t="n">
-        <v>45890.5</v>
+        <v>45892.5</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>SELL_VOLUME</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>2.901066174357815</v>
+        <v>3.059550124367895</v>
       </c>
       <c r="E175" t="n">
-        <v>-1.735697737521566</v>
+        <v>3.309120761518586</v>
       </c>
       <c r="F175" t="n">
-        <v>-0.0009501258603874518</v>
+        <v>0.02123466475467994</v>
       </c>
       <c r="G175" t="n">
-        <v>0.007367844180052161</v>
+        <v>0.004499636166002064</v>
       </c>
       <c r="H175" t="n">
-        <v>-228659661.1411896</v>
+        <v>-123132194.8514957</v>
       </c>
       <c r="I175" t="n">
-        <v>-0.4408405543264862</v>
+        <v>1.032363633766611</v>
       </c>
       <c r="J175" t="n">
         <v>1</v>
@@ -47555,7 +47279,7 @@
         </is>
       </c>
       <c r="B176" s="2" t="n">
-        <v>45891.5</v>
+        <v>45902.5</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -47563,22 +47287,22 @@
         </is>
       </c>
       <c r="D176" t="n">
-        <v>2.961548895020256</v>
+        <v>2.806723591636079</v>
       </c>
       <c r="E176" t="n">
         <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>0.02251244456848189</v>
+        <v>0.01420647421846422</v>
       </c>
       <c r="G176" t="n">
-        <v>0.006040177084133864</v>
+        <v>0.006650164733717385</v>
       </c>
       <c r="H176" t="n">
-        <v>349435963.2458496</v>
+        <v>445569893.2843523</v>
       </c>
       <c r="I176" t="n">
-        <v>0.9160404318878156</v>
+        <v>0.4968932840220217</v>
       </c>
       <c r="J176" t="n">
         <v>1</v>
@@ -47597,7 +47321,7 @@
         </is>
       </c>
       <c r="B177" s="2" t="n">
-        <v>45892.5</v>
+        <v>45903.5</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -47605,22 +47329,22 @@
         </is>
       </c>
       <c r="D177" t="n">
-        <v>3.059550124367895</v>
+        <v>2.852681735633498</v>
       </c>
       <c r="E177" t="n">
-        <v>3.309120761518586</v>
+        <v>1.637430352399929</v>
       </c>
       <c r="F177" t="n">
-        <v>0.02123466475467994</v>
+        <v>0.01274604448192074</v>
       </c>
       <c r="G177" t="n">
-        <v>0.004499636166002064</v>
+        <v>0.008738267994225928</v>
       </c>
       <c r="H177" t="n">
-        <v>-123132194.8514957</v>
+        <v>-281668949.5671759</v>
       </c>
       <c r="I177" t="n">
-        <v>1.032363633766611</v>
+        <v>0.2600654786251684</v>
       </c>
       <c r="J177" t="n">
         <v>1</v>
@@ -47629,90 +47353,6 @@
         <v>1400</v>
       </c>
       <c r="L177" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>XRP</t>
-        </is>
-      </c>
-      <c r="B178" s="2" t="n">
-        <v>45902.5</v>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D178" t="n">
-        <v>2.806723591636079</v>
-      </c>
-      <c r="E178" t="n">
-        <v>0</v>
-      </c>
-      <c r="F178" t="n">
-        <v>0.01420647421846422</v>
-      </c>
-      <c r="G178" t="n">
-        <v>0.006650164733717385</v>
-      </c>
-      <c r="H178" t="n">
-        <v>445569893.2843523</v>
-      </c>
-      <c r="I178" t="n">
-        <v>0.4968932840220217</v>
-      </c>
-      <c r="J178" t="n">
-        <v>1</v>
-      </c>
-      <c r="K178" t="n">
-        <v>1400</v>
-      </c>
-      <c r="L178" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>XRP</t>
-        </is>
-      </c>
-      <c r="B179" s="2" t="n">
-        <v>45903.5</v>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>SELL_VOLUME</t>
-        </is>
-      </c>
-      <c r="D179" t="n">
-        <v>2.852681735633498</v>
-      </c>
-      <c r="E179" t="n">
-        <v>1.637430352399929</v>
-      </c>
-      <c r="F179" t="n">
-        <v>0.01274604448192074</v>
-      </c>
-      <c r="G179" t="n">
-        <v>0.008738267994225928</v>
-      </c>
-      <c r="H179" t="n">
-        <v>-281668949.5671759</v>
-      </c>
-      <c r="I179" t="n">
-        <v>0.2600654786251684</v>
-      </c>
-      <c r="J179" t="n">
-        <v>1</v>
-      </c>
-      <c r="K179" t="n">
-        <v>1400</v>
-      </c>
-      <c r="L179" t="n">
         <v>20</v>
       </c>
     </row>
@@ -47727,7 +47367,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56077,19 +55717,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>0.4924489920051195</v>
+        <v>0.48871316690024</v>
       </c>
       <c r="C182" t="n">
-        <v>0.0008858576706284871</v>
+        <v>0.0001075607737785478</v>
       </c>
       <c r="D182" t="n">
-        <v>0.00090656170191664</v>
+        <v>0.0008751358967842345</v>
       </c>
       <c r="E182" t="n">
-        <v>-12344107.44526947</v>
+        <v>-10171624.05697095</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -56106,7 +55746,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.004796648973730332</v>
+        <v>-0.178282447233844</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -56118,52 +55758,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>0.48871316690024</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-8.129096763292987e-05</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.0005268421924038084</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-1869786.335683107</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.150850691457146</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>
@@ -57189,7 +56783,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -65539,19 +65133,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>110479.5500242308</v>
+        <v>110209.1888247784</v>
       </c>
       <c r="C182" t="n">
-        <v>4.924997417751001</v>
+        <v>-51.40025246817095</v>
       </c>
       <c r="D182" t="n">
-        <v>135.4516536861403</v>
+        <v>133.6814239948167</v>
       </c>
       <c r="E182" t="n">
-        <v>-2930032754.083179</v>
+        <v>-2958891210.070526</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -65568,7 +65162,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.5051544920221954</v>
+        <v>-0.7156949594445039</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -65580,52 +65174,6 @@
         <v>40</v>
       </c>
       <c r="N182" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>110209.1888247784</v>
-      </c>
-      <c r="C183" t="n">
-        <v>-49.81916741549503</v>
-      </c>
-      <c r="D183" t="n">
-        <v>132.1202441612651</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-1474083258.61882</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.7039810285341946</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>2800</v>
-      </c>
-      <c r="M183" t="n">
-        <v>40</v>
-      </c>
-      <c r="N183" t="n">
         <v>40</v>
       </c>
     </row>
@@ -66743,7 +66291,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -75093,19 +74641,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>4292.573365594387</v>
+        <v>4273.110024157841</v>
       </c>
       <c r="C182" t="n">
-        <v>4.090981767420089</v>
+        <v>0.0361189681398173</v>
       </c>
       <c r="D182" t="n">
-        <v>2.933237868030957</v>
+        <v>2.765960606625027</v>
       </c>
       <c r="E182" t="n">
-        <v>-1862009037.001507</v>
+        <v>-1869285302.825317</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -75122,7 +74670,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>0.05974426481824494</v>
+        <v>-0.1413393381787935</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -75134,52 +74682,6 @@
         <v>25</v>
       </c>
       <c r="N182" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>4273.110024157841</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.08273872573045082</v>
-      </c>
-      <c r="D183" t="n">
-        <v>2.234326172254721</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-864856988.2860146</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.113341312372159</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>1750</v>
-      </c>
-      <c r="M183" t="n">
-        <v>25</v>
-      </c>
-      <c r="N183" t="n">
         <v>25</v>
       </c>
     </row>
@@ -76205,7 +75707,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -84555,19 +84057,19 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45907.04166666666</v>
+        <v>45907.5</v>
       </c>
       <c r="B182" t="n">
-        <v>2.4183823206319</v>
+        <v>2.401956105970934</v>
       </c>
       <c r="C182" t="n">
-        <v>0.005578600301867187</v>
+        <v>0.002156472247499153</v>
       </c>
       <c r="D182" t="n">
-        <v>0.005966897235482153</v>
+        <v>0.005832441460763272</v>
       </c>
       <c r="E182" t="n">
-        <v>-6115665.640589029</v>
+        <v>-6868181.216256693</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -84584,7 +84086,7 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>-0.02947731154665068</v>
+        <v>-0.2799252041075787</v>
       </c>
       <c r="K182" t="n">
         <v>1</v>
@@ -84596,52 +84098,6 @@
         <v>10</v>
       </c>
       <c r="N182" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
-        <v>45907.5</v>
-      </c>
-      <c r="B183" t="n">
-        <v>2.401956105970934</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0.0003065529352817009</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.005224299736586062</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-3236099.145264819</v>
-      </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="G183" t="b">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>-0.3850896419214736</v>
-      </c>
-      <c r="K183" t="n">
-        <v>1</v>
-      </c>
-      <c r="L183" t="n">
-        <v>700</v>
-      </c>
-      <c r="M183" t="n">
-        <v>10</v>
-      </c>
-      <c r="N183" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>